<commit_message>
ya se añaden los tokens excepto d sets y actions
</commit_message>
<xml_diff>
--- a/arbol_expression_follows.xlsx
+++ b/arbol_expression_follows.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
   <si>
     <t>SÍMBOLO</t>
   </si>
@@ -23,40 +23,166 @@
     <t>[2, 3]</t>
   </si>
   <si>
-    <t>[23]</t>
+    <t>[90]</t>
   </si>
   <si>
     <t>[5]</t>
   </si>
   <si>
-    <t>[7]</t>
+    <t>[6]</t>
+  </si>
+  <si>
+    <t>[10]</t>
   </si>
   <si>
     <t>[8]</t>
   </si>
   <si>
-    <t>[10]</t>
-  </si>
-  <si>
-    <t>[12]</t>
-  </si>
-  <si>
-    <t>[14]</t>
+    <t>[9]</t>
+  </si>
+  <si>
+    <t>[12, 13, 14]</t>
   </si>
   <si>
     <t>[15]</t>
   </si>
   <si>
+    <t>[16]</t>
+  </si>
+  <si>
     <t>[17]</t>
   </si>
   <si>
-    <t>[18]</t>
-  </si>
-  <si>
-    <t>[20]</t>
+    <t>[19]</t>
+  </si>
+  <si>
+    <t>[21]</t>
   </si>
   <si>
     <t>[22]</t>
+  </si>
+  <si>
+    <t>[24]</t>
+  </si>
+  <si>
+    <t>[26]</t>
+  </si>
+  <si>
+    <t>[28]</t>
+  </si>
+  <si>
+    <t>[29]</t>
+  </si>
+  <si>
+    <t>[31]</t>
+  </si>
+  <si>
+    <t>[32]</t>
+  </si>
+  <si>
+    <t>[34]</t>
+  </si>
+  <si>
+    <t>[36]</t>
+  </si>
+  <si>
+    <t>[38]</t>
+  </si>
+  <si>
+    <t>[39]</t>
+  </si>
+  <si>
+    <t>[41]</t>
+  </si>
+  <si>
+    <t>[43]</t>
+  </si>
+  <si>
+    <t>[44]</t>
+  </si>
+  <si>
+    <t>[45]</t>
+  </si>
+  <si>
+    <t>[47]</t>
+  </si>
+  <si>
+    <t>[48]</t>
+  </si>
+  <si>
+    <t>[49]</t>
+  </si>
+  <si>
+    <t>[51]</t>
+  </si>
+  <si>
+    <t>[52]</t>
+  </si>
+  <si>
+    <t>[53]</t>
+  </si>
+  <si>
+    <t>[55]</t>
+  </si>
+  <si>
+    <t>[56]</t>
+  </si>
+  <si>
+    <t>[57]</t>
+  </si>
+  <si>
+    <t>[59]</t>
+  </si>
+  <si>
+    <t>[60]</t>
+  </si>
+  <si>
+    <t>[62]</t>
+  </si>
+  <si>
+    <t>[63]</t>
+  </si>
+  <si>
+    <t>[65]</t>
+  </si>
+  <si>
+    <t>[67]</t>
+  </si>
+  <si>
+    <t>[69]</t>
+  </si>
+  <si>
+    <t>[71]</t>
+  </si>
+  <si>
+    <t>[73]</t>
+  </si>
+  <si>
+    <t>[75]</t>
+  </si>
+  <si>
+    <t>[77]</t>
+  </si>
+  <si>
+    <t>[79]</t>
+  </si>
+  <si>
+    <t>[81]</t>
+  </si>
+  <si>
+    <t>[82]</t>
+  </si>
+  <si>
+    <t>[84]</t>
+  </si>
+  <si>
+    <t>[86]</t>
+  </si>
+  <si>
+    <t>[88]</t>
+  </si>
+  <si>
+    <t>[89]</t>
   </si>
 </sst>
 </file>
@@ -117,7 +243,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B90"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -168,7 +294,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -176,7 +302,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -184,7 +310,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -192,7 +318,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -200,7 +326,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -216,7 +342,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
@@ -224,7 +350,7 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
@@ -248,7 +374,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17">
@@ -256,7 +382,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
@@ -264,7 +390,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -272,7 +398,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20">
@@ -280,7 +406,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -288,7 +414,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
@@ -296,7 +422,7 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
@@ -304,6 +430,542 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="B65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="B67" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67.0</v>
+      </c>
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68.0</v>
+      </c>
+      <c r="B69" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="B71" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="B73" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73.0</v>
+      </c>
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74.0</v>
+      </c>
+      <c r="B75" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76.0</v>
+      </c>
+      <c r="B77" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="B78" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78.0</v>
+      </c>
+      <c r="B79" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79.0</v>
+      </c>
+      <c r="B80" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="B81" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81.0</v>
+      </c>
+      <c r="B82" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83.0</v>
+      </c>
+      <c r="B84" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84.0</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="B86" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86.0</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="B88" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88.0</v>
+      </c>
+      <c r="B89" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89.0</v>
+      </c>
+      <c r="B90" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se aceptan los sets
</commit_message>
<xml_diff>
--- a/arbol_expression_follows.xlsx
+++ b/arbol_expression_follows.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t>SÍMBOLO</t>
   </si>
@@ -23,7 +23,7 @@
     <t>[2, 3]</t>
   </si>
   <si>
-    <t>[90]</t>
+    <t>[88]</t>
   </si>
   <si>
     <t>[5]</t>
@@ -41,22 +41,19 @@
     <t>[9]</t>
   </si>
   <si>
-    <t>[12, 13, 14]</t>
+    <t>[12, 13, 15]</t>
   </si>
   <si>
     <t>[15]</t>
   </si>
   <si>
-    <t>[16]</t>
-  </si>
-  <si>
     <t>[17]</t>
   </si>
   <si>
     <t>[19]</t>
   </si>
   <si>
-    <t>[21]</t>
+    <t>[20]</t>
   </si>
   <si>
     <t>[22]</t>
@@ -68,13 +65,13 @@
     <t>[26]</t>
   </si>
   <si>
-    <t>[28]</t>
+    <t>[27]</t>
   </si>
   <si>
     <t>[29]</t>
   </si>
   <si>
-    <t>[31]</t>
+    <t>[30]</t>
   </si>
   <si>
     <t>[32]</t>
@@ -86,7 +83,7 @@
     <t>[36]</t>
   </si>
   <si>
-    <t>[38]</t>
+    <t>[37]</t>
   </si>
   <si>
     <t>[39]</t>
@@ -95,49 +92,49 @@
     <t>[41]</t>
   </si>
   <si>
+    <t>[42]</t>
+  </si>
+  <si>
     <t>[43]</t>
   </si>
   <si>
-    <t>[44]</t>
-  </si>
-  <si>
     <t>[45]</t>
   </si>
   <si>
+    <t>[46]</t>
+  </si>
+  <si>
     <t>[47]</t>
   </si>
   <si>
-    <t>[48]</t>
-  </si>
-  <si>
     <t>[49]</t>
   </si>
   <si>
+    <t>[50]</t>
+  </si>
+  <si>
     <t>[51]</t>
   </si>
   <si>
-    <t>[52]</t>
-  </si>
-  <si>
     <t>[53]</t>
   </si>
   <si>
+    <t>[54]</t>
+  </si>
+  <si>
     <t>[55]</t>
   </si>
   <si>
-    <t>[56]</t>
-  </si>
-  <si>
     <t>[57]</t>
   </si>
   <si>
-    <t>[59]</t>
+    <t>[58]</t>
   </si>
   <si>
     <t>[60]</t>
   </si>
   <si>
-    <t>[62]</t>
+    <t>[61]</t>
   </si>
   <si>
     <t>[63]</t>
@@ -167,7 +164,7 @@
     <t>[79]</t>
   </si>
   <si>
-    <t>[81]</t>
+    <t>[80]</t>
   </si>
   <si>
     <t>[82]</t>
@@ -179,10 +176,7 @@
     <t>[86]</t>
   </si>
   <si>
-    <t>[88]</t>
-  </si>
-  <si>
-    <t>[89]</t>
+    <t>[87]</t>
   </si>
 </sst>
 </file>
@@ -243,7 +237,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -374,7 +368,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -382,7 +376,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18">
@@ -398,7 +392,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -406,7 +400,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21">
@@ -414,7 +408,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
@@ -422,7 +416,7 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
@@ -438,7 +432,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25">
@@ -454,7 +448,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27">
@@ -462,7 +456,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28">
@@ -470,7 +464,7 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
@@ -478,7 +472,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30">
@@ -486,7 +480,7 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31">
@@ -494,7 +488,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
@@ -502,7 +496,7 @@
         <v>31.0</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33">
@@ -518,7 +512,7 @@
         <v>33.0</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35">
@@ -534,7 +528,7 @@
         <v>35.0</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37">
@@ -542,7 +536,7 @@
         <v>36.0</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38">
@@ -550,7 +544,7 @@
         <v>37.0</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -558,7 +552,7 @@
         <v>38.0</v>
       </c>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40">
@@ -574,7 +568,7 @@
         <v>40.0</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42">
@@ -582,7 +576,7 @@
         <v>41.0</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43">
@@ -598,7 +592,7 @@
         <v>43.0</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
@@ -606,7 +600,7 @@
         <v>44.0</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46">
@@ -614,7 +608,7 @@
         <v>45.0</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47">
@@ -630,7 +624,7 @@
         <v>47.0</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
@@ -638,7 +632,7 @@
         <v>48.0</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50">
@@ -646,7 +640,7 @@
         <v>49.0</v>
       </c>
       <c r="B50" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51">
@@ -662,7 +656,7 @@
         <v>51.0</v>
       </c>
       <c r="B52" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53">
@@ -670,7 +664,7 @@
         <v>52.0</v>
       </c>
       <c r="B53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54">
@@ -678,7 +672,7 @@
         <v>53.0</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55">
@@ -694,7 +688,7 @@
         <v>55.0</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
@@ -702,7 +696,7 @@
         <v>56.0</v>
       </c>
       <c r="B57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58">
@@ -710,7 +704,7 @@
         <v>57.0</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59">
@@ -718,7 +712,7 @@
         <v>58.0</v>
       </c>
       <c r="B59" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
@@ -726,7 +720,7 @@
         <v>59.0</v>
       </c>
       <c r="B60" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61">
@@ -734,7 +728,7 @@
         <v>60.0</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="62">
@@ -742,7 +736,7 @@
         <v>61.0</v>
       </c>
       <c r="B62" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63">
@@ -750,7 +744,7 @@
         <v>62.0</v>
       </c>
       <c r="B63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64">
@@ -766,7 +760,7 @@
         <v>64.0</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66">
@@ -782,7 +776,7 @@
         <v>66.0</v>
       </c>
       <c r="B67" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68">
@@ -798,7 +792,7 @@
         <v>68.0</v>
       </c>
       <c r="B69" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70">
@@ -814,7 +808,7 @@
         <v>70.0</v>
       </c>
       <c r="B71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72">
@@ -830,7 +824,7 @@
         <v>72.0</v>
       </c>
       <c r="B73" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74">
@@ -846,7 +840,7 @@
         <v>74.0</v>
       </c>
       <c r="B75" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="76">
@@ -862,7 +856,7 @@
         <v>76.0</v>
       </c>
       <c r="B77" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="78">
@@ -878,7 +872,7 @@
         <v>78.0</v>
       </c>
       <c r="B79" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="80">
@@ -886,7 +880,7 @@
         <v>79.0</v>
       </c>
       <c r="B80" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
     </row>
     <row r="81">
@@ -894,7 +888,7 @@
         <v>80.0</v>
       </c>
       <c r="B81" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82">
@@ -902,7 +896,7 @@
         <v>81.0</v>
       </c>
       <c r="B82" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="83">
@@ -918,7 +912,7 @@
         <v>83.0</v>
       </c>
       <c r="B84" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="85">
@@ -934,7 +928,7 @@
         <v>85.0</v>
       </c>
       <c r="B86" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="87">
@@ -942,7 +936,7 @@
         <v>86.0</v>
       </c>
       <c r="B87" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
     </row>
     <row r="88">
@@ -950,22 +944,6 @@
         <v>87.0</v>
       </c>
       <c r="B88" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>88.0</v>
-      </c>
-      <c r="B89" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>89.0</v>
-      </c>
-      <c r="B90" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se modificaron varias cosas
</commit_message>
<xml_diff>
--- a/arbol_expression_follows.xlsx
+++ b/arbol_expression_follows.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
   <si>
     <t>SÍMBOLO</t>
   </si>
@@ -23,160 +23,160 @@
     <t>[2, 3]</t>
   </si>
   <si>
+    <t>[89]</t>
+  </si>
+  <si>
+    <t>[5]</t>
+  </si>
+  <si>
+    <t>[6]</t>
+  </si>
+  <si>
+    <t>[10]</t>
+  </si>
+  <si>
+    <t>[8]</t>
+  </si>
+  <si>
+    <t>[9]</t>
+  </si>
+  <si>
+    <t>[12, 13, 15]</t>
+  </si>
+  <si>
+    <t>[15]</t>
+  </si>
+  <si>
+    <t>[17]</t>
+  </si>
+  <si>
+    <t>[19]</t>
+  </si>
+  <si>
+    <t>[20]</t>
+  </si>
+  <si>
+    <t>[22]</t>
+  </si>
+  <si>
+    <t>[24]</t>
+  </si>
+  <si>
+    <t>[26]</t>
+  </si>
+  <si>
+    <t>[27]</t>
+  </si>
+  <si>
+    <t>[29]</t>
+  </si>
+  <si>
+    <t>[30]</t>
+  </si>
+  <si>
+    <t>[32]</t>
+  </si>
+  <si>
+    <t>[34]</t>
+  </si>
+  <si>
+    <t>[36]</t>
+  </si>
+  <si>
+    <t>[37]</t>
+  </si>
+  <si>
+    <t>[39]</t>
+  </si>
+  <si>
+    <t>[41]</t>
+  </si>
+  <si>
+    <t>[42]</t>
+  </si>
+  <si>
+    <t>[43]</t>
+  </si>
+  <si>
+    <t>[45]</t>
+  </si>
+  <si>
+    <t>[46]</t>
+  </si>
+  <si>
+    <t>[47]</t>
+  </si>
+  <si>
+    <t>[49]</t>
+  </si>
+  <si>
+    <t>[50]</t>
+  </si>
+  <si>
+    <t>[51]</t>
+  </si>
+  <si>
+    <t>[53]</t>
+  </si>
+  <si>
+    <t>[54]</t>
+  </si>
+  <si>
+    <t>[55]</t>
+  </si>
+  <si>
+    <t>[57]</t>
+  </si>
+  <si>
+    <t>[58]</t>
+  </si>
+  <si>
+    <t>[60]</t>
+  </si>
+  <si>
+    <t>[61]</t>
+  </si>
+  <si>
+    <t>[63]</t>
+  </si>
+  <si>
+    <t>[65]</t>
+  </si>
+  <si>
+    <t>[67]</t>
+  </si>
+  <si>
+    <t>[69]</t>
+  </si>
+  <si>
+    <t>[71]</t>
+  </si>
+  <si>
+    <t>[73]</t>
+  </si>
+  <si>
+    <t>[75]</t>
+  </si>
+  <si>
+    <t>[77]</t>
+  </si>
+  <si>
+    <t>[79]</t>
+  </si>
+  <si>
+    <t>[80]</t>
+  </si>
+  <si>
+    <t>[82]</t>
+  </si>
+  <si>
+    <t>[84]</t>
+  </si>
+  <si>
+    <t>[86]</t>
+  </si>
+  <si>
     <t>[88]</t>
-  </si>
-  <si>
-    <t>[5]</t>
-  </si>
-  <si>
-    <t>[6]</t>
-  </si>
-  <si>
-    <t>[10]</t>
-  </si>
-  <si>
-    <t>[8]</t>
-  </si>
-  <si>
-    <t>[9]</t>
-  </si>
-  <si>
-    <t>[12, 13, 15]</t>
-  </si>
-  <si>
-    <t>[15]</t>
-  </si>
-  <si>
-    <t>[17]</t>
-  </si>
-  <si>
-    <t>[19]</t>
-  </si>
-  <si>
-    <t>[20]</t>
-  </si>
-  <si>
-    <t>[22]</t>
-  </si>
-  <si>
-    <t>[24]</t>
-  </si>
-  <si>
-    <t>[26]</t>
-  </si>
-  <si>
-    <t>[27]</t>
-  </si>
-  <si>
-    <t>[29]</t>
-  </si>
-  <si>
-    <t>[30]</t>
-  </si>
-  <si>
-    <t>[32]</t>
-  </si>
-  <si>
-    <t>[34]</t>
-  </si>
-  <si>
-    <t>[36]</t>
-  </si>
-  <si>
-    <t>[37]</t>
-  </si>
-  <si>
-    <t>[39]</t>
-  </si>
-  <si>
-    <t>[41]</t>
-  </si>
-  <si>
-    <t>[42]</t>
-  </si>
-  <si>
-    <t>[43]</t>
-  </si>
-  <si>
-    <t>[45]</t>
-  </si>
-  <si>
-    <t>[46]</t>
-  </si>
-  <si>
-    <t>[47]</t>
-  </si>
-  <si>
-    <t>[49]</t>
-  </si>
-  <si>
-    <t>[50]</t>
-  </si>
-  <si>
-    <t>[51]</t>
-  </si>
-  <si>
-    <t>[53]</t>
-  </si>
-  <si>
-    <t>[54]</t>
-  </si>
-  <si>
-    <t>[55]</t>
-  </si>
-  <si>
-    <t>[57]</t>
-  </si>
-  <si>
-    <t>[58]</t>
-  </si>
-  <si>
-    <t>[60]</t>
-  </si>
-  <si>
-    <t>[61]</t>
-  </si>
-  <si>
-    <t>[63]</t>
-  </si>
-  <si>
-    <t>[65]</t>
-  </si>
-  <si>
-    <t>[67]</t>
-  </si>
-  <si>
-    <t>[69]</t>
-  </si>
-  <si>
-    <t>[71]</t>
-  </si>
-  <si>
-    <t>[73]</t>
-  </si>
-  <si>
-    <t>[75]</t>
-  </si>
-  <si>
-    <t>[77]</t>
-  </si>
-  <si>
-    <t>[79]</t>
-  </si>
-  <si>
-    <t>[80]</t>
-  </si>
-  <si>
-    <t>[82]</t>
-  </si>
-  <si>
-    <t>[84]</t>
-  </si>
-  <si>
-    <t>[86]</t>
-  </si>
-  <si>
-    <t>[87]</t>
   </si>
 </sst>
 </file>
@@ -237,7 +237,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -944,6 +944,14 @@
         <v>87.0</v>
       </c>
       <c r="B88" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88.0</v>
+      </c>
+      <c r="B89" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>